<commit_message>
create chart from data FINAL@
</commit_message>
<xml_diff>
--- a/excel/excel_layout.xlsx
+++ b/excel/excel_layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\natashaval\qubit-mapping-distributed-qc\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC7914A-5D83-4179-B80B-45A77AE1AB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C736A3-3BA3-40E2-8AF9-4E5DCA614156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4021,7 +4021,7 @@
   <dimension ref="A1:U138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>